<commit_message>
Add web app, update ignore rules, remove nested git repo
</commit_message>
<xml_diff>
--- a/attendance.csv.xlsx
+++ b/attendance.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartAttendance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{494E5D01-36E6-4A25-81A4-82E0C4A82736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE851023-B758-46E0-B593-AC61BEA6F77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9420" xr2:uid="{A95F5739-B866-49B5-84D5-CEE30BD85433}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="9420" xr2:uid="{11C14AA4-9329-45E1-99A1-C85861967789}"/>
   </bookViews>
   <sheets>
     <sheet name="attendance" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Name</t>
   </si>
@@ -29,12 +29,6 @@
   </si>
   <si>
     <t>Time</t>
-  </si>
-  <si>
-    <t>Yash</t>
-  </si>
-  <si>
-    <t>Ansh</t>
   </si>
 </sst>
 </file>
@@ -876,10 +870,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017C3083-2A59-4E4F-9702-3350ACA1FDF6}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C02E84-6AB3-4285-9800-66C5EF43D9C7}">
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -894,27 +890,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45927</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1.9444444444444445E-2</v>
-      </c>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45927</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2.1539351851851851E-2</v>
-      </c>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>